<commit_message>
bf: update tas3 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2024/oct/bf_lf_tas3_2410_2_fts.xlsx
+++ b/LF/TAS/Burkina Faso/2024/oct/bf_lf_tas3_2410_2_fts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\oct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D22F4D-D3B7-4280-8BD7-FEA9C605C527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44078292-62F9-41CA-A6E4-A366B67126F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="181">
   <si>
     <t>type</t>
   </si>
@@ -69,9 +69,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>select_one d_id_type</t>
   </si>
   <si>
@@ -372,12 +369,6 @@
     <t>control_list</t>
   </si>
   <si>
-    <t>Lot1: 238429 Exp : 30/05/2024</t>
-  </si>
-  <si>
-    <t>Lot2: 766673A Exp : 10/08/2024</t>
-  </si>
-  <si>
     <t>EN09</t>
   </si>
   <si>
@@ -390,15 +381,6 @@
     <t>EN12</t>
   </si>
   <si>
-    <t>bf_lf_tas3_2410_2_fts</t>
-  </si>
-  <si>
-    <t>(Oct 2024) Burkina Faso TAS3 - 2. Formulaire Résultats</t>
-  </si>
-  <si>
-    <t>d_ds</t>
-  </si>
-  <si>
     <t>c_nom_CSPS</t>
   </si>
   <si>
@@ -505,9 +487,6 @@
   </si>
   <si>
     <t>Vous venez de saisir une valeur qui mettra fin à l'enquête</t>
-  </si>
-  <si>
-    <t>bf_tas_f_2410</t>
   </si>
   <si>
     <t>end repeat</t>
@@ -584,6 +563,24 @@
   </si>
   <si>
     <t>d_num_grappe</t>
+  </si>
+  <si>
+    <t>bf_lf_tas3_2410_2_fts_v2</t>
+  </si>
+  <si>
+    <t>(Oct 2024) Burkina Faso TAS3 - 2. Formulaire Résultats V2</t>
+  </si>
+  <si>
+    <t>bf_tas_f_24102</t>
+  </si>
+  <si>
+    <t>Lot1: 838060 Exp : 24/01/2025</t>
+  </si>
+  <si>
+    <t>d_ue</t>
+  </si>
+  <si>
+    <t>UE</t>
   </si>
 </sst>
 </file>
@@ -794,16 +791,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -846,8 +839,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -861,8 +854,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,7 +1290,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="15.75">
@@ -1304,248 +1301,248 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="19" customFormat="1" ht="15.75">
+    <row r="3" spans="1:13" s="17" customFormat="1" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75">
-      <c r="A4" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="J4" s="21" t="s">
+      <c r="A4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="J4" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>181</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="15.75">
       <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="15.75">
+      <c r="A7" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="1:13" s="6" customFormat="1" ht="15.75">
+      <c r="A8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B8" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="15.75">
+      <c r="A9" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="15.75">
-      <c r="A7" s="22" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="15.75">
+      <c r="A10" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="15.75">
-      <c r="A8" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="33"/>
-    </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="15.75">
-      <c r="A9" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="23" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="15.75">
-      <c r="A10" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="15.75">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="15.75">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="15.75">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="F13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75">
-      <c r="A14" s="21" t="s">
-        <v>22</v>
+      <c r="A14" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>14</v>
@@ -1553,351 +1550,351 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>142</v>
+        <v>21</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>163</v>
+        <v>133</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A16" s="34" t="s">
+    <row r="16" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A16" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="C16" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="B17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A18" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A19" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A20" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="33" customFormat="1" ht="15.75">
+      <c r="A21" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A22" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A23" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="H23" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A17" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="34" t="s">
+    <row r="24" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A24" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H24" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I24" s="32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A18" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="34" t="s">
+    <row r="25" spans="1:13" s="33" customFormat="1" ht="15.75">
+      <c r="A25" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="H18" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="I18" s="34" t="s">
+      <c r="D25" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A19" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="34" t="s">
+    <row r="26" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A26" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A27" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="34" t="s">
+      <c r="B27" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="162.75" customHeight="1">
+      <c r="A28" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="20"/>
+      <c r="J28" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+    </row>
+    <row r="29" spans="1:13" s="19" customFormat="1" ht="31.5">
+      <c r="A29" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="I19" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A20" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="35" customFormat="1" ht="15.75">
-      <c r="A21" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A22" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="34" t="s">
+      <c r="D29" s="39"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+    </row>
+    <row r="30" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A30" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A23" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="34" t="s">
+      <c r="H30" s="32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="32" customFormat="1" ht="15.75">
+      <c r="A31" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="6" customFormat="1" ht="15.75">
+      <c r="A32" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="H23" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="I23" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A24" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="I24" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="35" customFormat="1" ht="15.75">
-      <c r="A25" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A26" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A27" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="I27" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="162.75" customHeight="1">
-      <c r="A28" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="22"/>
-      <c r="J28" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-    </row>
-    <row r="29" spans="1:13" s="21" customFormat="1" ht="31.5">
-      <c r="A29" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-    </row>
-    <row r="30" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A30" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="34" customFormat="1" ht="15.75">
-      <c r="A31" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="6" customFormat="1" ht="15.75">
-      <c r="A32" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="33"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="31"/>
     </row>
     <row r="33" spans="1:2" s="1" customFormat="1" ht="15.75">
       <c r="A33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="1" customFormat="1" ht="15.75">
       <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="35" spans="1:2" s="1" customFormat="1" ht="15.75"/>
-    <row r="36" spans="1:2" s="19" customFormat="1"/>
-    <row r="37" spans="1:2" s="19" customFormat="1"/>
-    <row r="38" spans="1:2" s="19" customFormat="1"/>
-    <row r="39" spans="1:2" s="19" customFormat="1"/>
-    <row r="40" spans="1:2" s="19" customFormat="1"/>
-    <row r="41" spans="1:2" s="19" customFormat="1"/>
-    <row r="42" spans="1:2" s="19" customFormat="1">
+    <row r="36" spans="1:2" s="17" customFormat="1"/>
+    <row r="37" spans="1:2" s="17" customFormat="1"/>
+    <row r="38" spans="1:2" s="17" customFormat="1"/>
+    <row r="39" spans="1:2" s="17" customFormat="1"/>
+    <row r="40" spans="1:2" s="17" customFormat="1"/>
+    <row r="41" spans="1:2" s="17" customFormat="1"/>
+    <row r="42" spans="1:2" s="17" customFormat="1">
       <c r="B42" s="12"/>
     </row>
-    <row r="43" spans="1:2" s="19" customFormat="1"/>
-    <row r="44" spans="1:2" s="19" customFormat="1"/>
+    <row r="43" spans="1:2" s="17" customFormat="1"/>
+    <row r="44" spans="1:2" s="17" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300"/>
@@ -1906,11 +1903,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1925,7 +1922,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1934,143 +1931,143 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="15.75">
@@ -2079,287 +2076,276 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>117</v>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="2">
-        <v>2</v>
-      </c>
-      <c r="C39" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2395,7 +2381,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2405,26 +2391,26 @@
     <col min="3" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" s="16" customFormat="1">
+      <c r="A1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>